<commit_message>
Added logic and row in datasheet for out of stock item
</commit_message>
<xml_diff>
--- a/20200529/Default.xlsx
+++ b/20200529/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>BusinessProcess</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>One</t>
+  </si>
+  <si>
+    <t>XL</t>
   </si>
   <si>
     <t>LastName</t>
@@ -541,7 +544,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
@@ -564,19 +567,19 @@
         <v>5</v>
       </c>
       <c t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c t="s">
         <v>3</v>
       </c>
       <c t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c t="s">
         <v>0</v>
       </c>
       <c t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c t="s">
         <v>2</v>
@@ -584,10 +587,10 @@
     </row>
     <row>
       <c s="1" t="s">
-        <v>10</v>
-      </c>
-      <c s="1" t="s">
         <v>11</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
       </c>
       <c s="1" t="s">
         <v>6</v>
@@ -603,10 +606,10 @@
     </row>
     <row>
       <c s="1" t="s">
-        <v>10</v>
-      </c>
-      <c s="1" t="s">
         <v>11</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
       </c>
       <c s="1" t="s">
         <v>6</v>
@@ -633,6 +636,21 @@
       </c>
       <c s="3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1"/>
+      <c s="1">
+        <v>3</v>
+      </c>
+      <c s="1" t="s">
+        <v>1</v>
+      </c>
+      <c s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>